<commit_message>
Removed crowd mics from split
</commit_message>
<xml_diff>
--- a/Input List/Acoustic/Input List.xlsx
+++ b/Input List/Acoustic/Input List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\TechnicalDocumentation\Input List\Acoustic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Input List\Acoustic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0B7E63-B91B-46FA-9255-0526D54BCE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E09C710-4ABD-45DD-B6C4-93AA59A5BCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Input + Equipment" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="64">
   <si>
     <t>Input</t>
   </si>
@@ -600,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -633,6 +633,29 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -657,8 +680,23 @@
     <xf numFmtId="0" fontId="7" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -672,82 +710,42 @@
     <xf numFmtId="0" fontId="2" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,9 +849,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -891,7 +889,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -997,7 +995,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1139,7 +1137,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1149,7 +1147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A11D25-D77D-4358-9E34-E04B11CA4C7B}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -1193,10 +1191,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="42" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="3">
@@ -1215,8 +1213,8 @@
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
-      <c r="B3" s="51"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="4">
         <v>2</v>
       </c>
@@ -1233,8 +1231,8 @@
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49"/>
-      <c r="B4" s="52"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="10">
         <v>3</v>
       </c>
@@ -1247,10 +1245,10 @@
       <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="32" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="13">
@@ -1269,8 +1267,8 @@
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="23"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="14">
         <v>5</v>
       </c>
@@ -1287,10 +1285,10 @@
       <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="36" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="8">
@@ -1309,8 +1307,8 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="28"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="9">
         <v>7</v>
       </c>
@@ -1327,8 +1325,8 @@
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="29"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="8">
         <v>8</v>
       </c>
@@ -1345,10 +1343,10 @@
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="47" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="11">
@@ -1367,8 +1365,8 @@
       <c r="H10" s="11"/>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="34"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="12">
         <v>10</v>
       </c>
@@ -1383,10 +1381,10 @@
       <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="26" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="5">
@@ -1405,8 +1403,8 @@
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
-      <c r="B13" s="54"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="6">
         <v>12</v>
       </c>
@@ -1423,8 +1421,8 @@
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
-      <c r="B14" s="55"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="5">
         <v>13</v>
       </c>
@@ -1441,68 +1439,68 @@
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="59">
+      <c r="C15" s="22">
         <v>14</v>
       </c>
-      <c r="D15" s="61" t="s">
+      <c r="D15" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="61" t="s">
+      <c r="E15" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="61" t="s">
+      <c r="F15" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="61" t="s">
+      <c r="G15" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="H15" s="61"/>
+      <c r="H15" s="22"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="57"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="60">
+      <c r="A16" s="29"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="23">
         <v>15</v>
       </c>
-      <c r="D16" s="62" t="s">
+      <c r="D16" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="62" t="s">
+      <c r="E16" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="62" t="s">
+      <c r="F16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="62" t="s">
+      <c r="G16" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="H16" s="62"/>
+      <c r="H16" s="23"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="58"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="59">
+      <c r="C17" s="22">
         <v>16</v>
       </c>
-      <c r="D17" s="59" t="s">
+      <c r="D17" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="59" t="s">
+      <c r="E17" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="59" t="s">
+      <c r="F17" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1541,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036672A4-8952-44C6-9E0D-0D4906E8D835}">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,33 +1559,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
       <c r="I1" s="19"/>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="44"/>
+      <c r="L1" s="56"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
       <c r="I2" s="19"/>
       <c r="K2" s="16" t="s">
         <v>11</v>
@@ -1632,26 +1630,26 @@
       <c r="O3" s="15"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="37" t="s">
+      <c r="C4" s="52"/>
+      <c r="D4" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="38" t="s">
+      <c r="H4" s="54" t="s">
         <v>43</v>
       </c>
       <c r="I4" s="19"/>
@@ -1664,14 +1662,14 @@
       <c r="O4" s="15"/>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
       <c r="I5" s="19"/>
       <c r="K5" s="16">
         <v>3</v>
@@ -1724,28 +1722,28 @@
       <c r="O7" s="15"/>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="46" t="s">
+      <c r="F8" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="46" t="s">
+      <c r="G8" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="46" t="s">
+      <c r="H8" s="49" t="s">
         <v>60</v>
       </c>
       <c r="I8" s="19"/>
@@ -1758,14 +1756,14 @@
       <c r="O8" s="15"/>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
       <c r="I9" s="19"/>
       <c r="K9" s="16">
         <v>7</v>
@@ -1786,16 +1784,16 @@
       <c r="O10" s="15"/>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
       <c r="I11" s="19"/>
       <c r="K11" s="16">
         <v>9</v>
@@ -1840,16 +1838,16 @@
       <c r="O12" s="15"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="46" t="s">
+      <c r="A13" s="52"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="46" t="s">
+      <c r="H13" s="49" t="s">
         <v>63</v>
       </c>
       <c r="I13" s="19"/>
@@ -1862,14 +1860,14 @@
       <c r="O13" s="15"/>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
+      <c r="A14" s="52"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
       <c r="I14" s="19"/>
       <c r="K14" s="16">
         <v>12</v>
@@ -1902,9 +1900,7 @@
       <c r="K16" s="16">
         <v>14</v>
       </c>
-      <c r="L16" s="16" t="s">
-        <v>55</v>
-      </c>
+      <c r="L16" s="16"/>
       <c r="O16" s="15"/>
     </row>
     <row r="17" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1912,9 +1908,7 @@
       <c r="K17" s="16">
         <v>15</v>
       </c>
-      <c r="L17" s="16" t="s">
-        <v>56</v>
-      </c>
+      <c r="L17" s="16"/>
       <c r="O17" s="15"/>
     </row>
     <row r="18" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1939,79 +1933,79 @@
     </row>
     <row r="21" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I21" s="19"/>
-      <c r="K21" s="45" t="s">
+      <c r="K21" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="45"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="57"/>
+      <c r="N21" s="57"/>
+      <c r="O21" s="57"/>
     </row>
     <row r="22" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I22" s="19"/>
       <c r="K22" s="7">
         <v>1</v>
       </c>
-      <c r="L22" s="42" t="s">
+      <c r="L22" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
+      <c r="M22" s="58"/>
+      <c r="N22" s="58"/>
+      <c r="O22" s="58"/>
     </row>
     <row r="23" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I23" s="19"/>
       <c r="K23" s="2">
         <v>2</v>
       </c>
-      <c r="L23" s="43" t="s">
+      <c r="L23" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="M23" s="43"/>
-      <c r="N23" s="43"/>
-      <c r="O23" s="43"/>
+      <c r="M23" s="59"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="59"/>
     </row>
     <row r="24" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I24" s="19"/>
       <c r="K24" s="7">
         <v>3</v>
       </c>
-      <c r="L24" s="42" t="s">
+      <c r="L24" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="58"/>
+      <c r="O24" s="58"/>
     </row>
     <row r="25" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I25" s="19"/>
       <c r="K25" s="2">
         <v>4</v>
       </c>
-      <c r="L25" s="43"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="43"/>
-      <c r="O25" s="43"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="59"/>
     </row>
     <row r="26" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I26" s="19"/>
       <c r="K26" s="7">
         <v>5</v>
       </c>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="58"/>
+      <c r="N26" s="58"/>
+      <c r="O26" s="58"/>
     </row>
     <row r="27" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I27" s="19"/>
       <c r="K27" s="2">
         <v>6</v>
       </c>
-      <c r="L27" s="43"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="43"/>
-      <c r="O27" s="43"/>
+      <c r="L27" s="59"/>
+      <c r="M27" s="59"/>
+      <c r="N27" s="59"/>
+      <c r="O27" s="59"/>
     </row>
     <row r="28" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2021,6 +2015,25 @@
     <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K21:O21"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="L24:O24"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="A11:H11"/>
@@ -2037,25 +2050,6 @@
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="K21:O21"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="L23:O23"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="L25:O25"/>
-    <mergeCell ref="L26:O26"/>
-    <mergeCell ref="L27:O27"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated descriptions, colors, and formatting
</commit_message>
<xml_diff>
--- a/Input List/Acoustic/Input List.xlsx
+++ b/Input List/Acoustic/Input List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Input List\Acoustic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7362C4-DACE-47D6-BAAA-08EAF0B45BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED9D0E0-347C-4FBD-A8C4-E19E40FFAF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Input + Equipment" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
   <si>
     <t>Input</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>All items will be on the floor</t>
+  </si>
+  <si>
+    <t>Light reverb. Light Delay</t>
+  </si>
+  <si>
+    <t>EQ up lower and mid. Lots of reverb.</t>
   </si>
 </sst>
 </file>
@@ -355,7 +361,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,12 +388,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -442,12 +442,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -460,12 +454,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00E266"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -488,8 +476,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -552,105 +546,30 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -660,125 +579,84 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -826,7 +704,13 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -835,12 +719,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -1180,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A11D25-D77D-4358-9E34-E04B11CA4C7B}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,56 +1076,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="18">
         <v>1</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="37"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="3">
         <v>2</v>
       </c>
@@ -1264,30 +1144,30 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="21">
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="18">
         <v>3</v>
       </c>
-      <c r="D4" s="61" t="s">
+      <c r="D4" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E4" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="61" t="s">
+      <c r="F4" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61" t="s">
+      <c r="G4" s="18"/>
+      <c r="H4" s="18" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="27" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="10">
@@ -1303,11 +1183,13 @@
         <v>13</v>
       </c>
       <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="H5" s="10" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="11">
         <v>5</v>
       </c>
@@ -1324,10 +1206,10 @@
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="29" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="7">
@@ -1343,11 +1225,13 @@
         <v>13</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28"/>
-      <c r="B8" s="31"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="8">
         <v>7</v>
       </c>
@@ -1364,8 +1248,8 @@
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="32"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="7">
         <v>8</v>
       </c>
@@ -1382,30 +1266,32 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="21">
         <v>9</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="42"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="9">
         <v>10</v>
       </c>
@@ -1422,10 +1308,10 @@
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="34" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="4">
@@ -1441,11 +1327,13 @@
         <v>30</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="5">
         <v>12</v>
       </c>
@@ -1462,8 +1350,8 @@
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="4">
         <v>13</v>
       </c>
@@ -1480,8 +1368,8 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
       <c r="C15" s="5">
         <v>14</v>
       </c>
@@ -1498,40 +1386,40 @@
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="57">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="19">
         <v>15</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="D16" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="60"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="55" t="s">
+      <c r="A17" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="20">
         <v>16</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1546,17 +1434,17 @@
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="D16:H16"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="D16:H16"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1568,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036672A4-8952-44C6-9E0D-0D4906E8D835}">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,322 +1476,322 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="16"/>
-      <c r="K1" s="48" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="15"/>
+      <c r="K1" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="48"/>
+      <c r="L1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="16"/>
-      <c r="K2" s="13" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="15"/>
+      <c r="K2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="22" t="s">
         <v>45</v>
       </c>
       <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="A3" s="14">
         <v>1</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <v>2</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>3</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>4</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>5</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="14">
         <v>6</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="14">
         <v>7</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="14">
         <v>8</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="K3" s="13">
+      <c r="I3" s="15"/>
+      <c r="K3" s="18">
         <v>1</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="O3" s="12"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="53" t="s">
+      <c r="G4" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="53" t="s">
+      <c r="H4" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="16"/>
-      <c r="K4" s="13">
+      <c r="I4" s="15"/>
+      <c r="K4" s="3">
         <v>2</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="3" t="s">
         <v>51</v>
       </c>
       <c r="O4" s="12"/>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="51"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="16"/>
-      <c r="K5" s="13">
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="15"/>
+      <c r="K5" s="18">
         <v>3</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="L5" s="18" t="s">
         <v>60</v>
       </c>
       <c r="O5" s="12"/>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I6" s="16"/>
-      <c r="K6" s="13">
+      <c r="I6" s="15"/>
+      <c r="K6" s="10">
         <v>4</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="L6" s="10" t="s">
         <v>34</v>
       </c>
       <c r="O6" s="12"/>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="A7" s="14">
         <v>9</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>10</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>11</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>12</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>13</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <v>14</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="14">
         <v>15</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <v>16</v>
       </c>
-      <c r="I7" s="16"/>
-      <c r="K7" s="13">
+      <c r="I7" s="15"/>
+      <c r="K7" s="11">
         <v>5</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="L7" s="11" t="s">
         <v>42</v>
       </c>
       <c r="O7" s="12"/>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="44"/>
-      <c r="H8" s="47" t="s">
+      <c r="G8" s="36"/>
+      <c r="H8" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="16"/>
-      <c r="K8" s="13">
+      <c r="I8" s="15"/>
+      <c r="K8" s="7">
         <v>6</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="L8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="O8" s="12"/>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="54"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="16"/>
-      <c r="K9" s="13">
+      <c r="A9" s="43"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="15"/>
+      <c r="K9" s="8">
         <v>7</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="8" t="s">
         <v>9</v>
       </c>
       <c r="O9" s="12"/>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I10" s="16"/>
-      <c r="K10" s="13">
+      <c r="I10" s="15"/>
+      <c r="K10" s="7">
         <v>8</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="7" t="s">
         <v>43</v>
       </c>
       <c r="O10" s="12"/>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="16"/>
-      <c r="K11" s="13">
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="15"/>
+      <c r="K11" s="21">
         <v>9</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="21" t="s">
         <v>1</v>
       </c>
       <c r="O11" s="12"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+      <c r="A12" s="14">
         <v>1</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>2</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>3</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <v>4</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="14">
         <v>5</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="14">
         <v>6</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="I12" s="16"/>
-      <c r="K12" s="13">
+      <c r="I12" s="15"/>
+      <c r="K12" s="9">
         <v>10</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="L12" s="9" t="s">
         <v>2</v>
       </c>
       <c r="O12" s="12"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="47" t="s">
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="47" t="s">
+      <c r="H13" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="I13" s="16"/>
-      <c r="K13" s="13">
+      <c r="I13" s="15"/>
+      <c r="K13" s="4">
         <v>11</v>
       </c>
-      <c r="L13" s="13" t="s">
+      <c r="L13" s="4" t="s">
         <v>3</v>
       </c>
       <c r="O13" s="12"/>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="16"/>
-      <c r="K14" s="13">
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="15"/>
+      <c r="K14" s="5">
         <v>12</v>
       </c>
-      <c r="L14" s="13" t="s">
+      <c r="L14" s="5" t="s">
         <v>32</v>
       </c>
       <c r="O14" s="12"/>
@@ -1917,47 +1805,51 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="16"/>
-      <c r="K15" s="13">
+      <c r="I15" s="15"/>
+      <c r="K15" s="4">
         <v>13</v>
       </c>
-      <c r="L15" s="13" t="s">
+      <c r="L15" s="4" t="s">
         <v>59</v>
       </c>
       <c r="O15" s="12"/>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I16" s="16"/>
-      <c r="K16" s="13">
+      <c r="I16" s="15"/>
+      <c r="K16" s="5">
         <v>14</v>
       </c>
-      <c r="L16" s="13" t="s">
+      <c r="L16" s="5" t="s">
         <v>4</v>
       </c>
       <c r="O16" s="12"/>
     </row>
     <row r="17" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I17" s="16"/>
-      <c r="K17" s="13">
+      <c r="I17" s="15"/>
+      <c r="K17" s="19">
         <v>15</v>
       </c>
-      <c r="L17" s="13"/>
+      <c r="L17" s="23" t="s">
+        <v>17</v>
+      </c>
       <c r="O17" s="12"/>
     </row>
     <row r="18" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I18" s="16"/>
-      <c r="K18" s="13">
+      <c r="I18" s="15"/>
+      <c r="K18" s="19">
         <v>16</v>
       </c>
-      <c r="L18" s="13"/>
+      <c r="L18" s="23" t="s">
+        <v>17</v>
+      </c>
       <c r="O18" s="12"/>
     </row>
     <row r="19" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I19" s="16"/>
+      <c r="I19" s="15"/>
     </row>
     <row r="20" spans="9:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I20" s="16"/>
-      <c r="J20" s="17"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="16"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -1965,17 +1857,17 @@
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I21" s="16"/>
-      <c r="K21" s="49" t="s">
+      <c r="I21" s="15"/>
+      <c r="K21" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="49"/>
-      <c r="O21" s="49"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="45"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="45"/>
     </row>
     <row r="22" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I22" s="16"/>
+      <c r="I22" s="15"/>
       <c r="K22" s="6">
         <v>1</v>
       </c>
@@ -1987,19 +1879,19 @@
       <c r="O22" s="46"/>
     </row>
     <row r="23" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I23" s="16"/>
+      <c r="I23" s="15"/>
       <c r="K23" s="2">
         <v>2</v>
       </c>
-      <c r="L23" s="45" t="s">
+      <c r="L23" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="M23" s="45"/>
-      <c r="N23" s="45"/>
-      <c r="O23" s="45"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="47"/>
     </row>
     <row r="24" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I24" s="16"/>
+      <c r="I24" s="15"/>
       <c r="K24" s="6">
         <v>3</v>
       </c>
@@ -2011,17 +1903,17 @@
       <c r="O24" s="46"/>
     </row>
     <row r="25" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I25" s="16"/>
+      <c r="I25" s="15"/>
       <c r="K25" s="2">
         <v>4</v>
       </c>
-      <c r="L25" s="45"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="45"/>
-      <c r="O25" s="45"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="47"/>
+      <c r="O25" s="47"/>
     </row>
     <row r="26" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I26" s="16"/>
+      <c r="I26" s="15"/>
       <c r="K26" s="6">
         <v>5</v>
       </c>
@@ -2031,14 +1923,14 @@
       <c r="O26" s="46"/>
     </row>
     <row r="27" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I27" s="16"/>
+      <c r="I27" s="15"/>
       <c r="K27" s="2">
         <v>6</v>
       </c>
-      <c r="L27" s="45"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="45"/>
+      <c r="L27" s="47"/>
+      <c r="M27" s="47"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="47"/>
     </row>
     <row r="28" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2048,6 +1940,25 @@
     <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K21:O21"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="L24:O24"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="A11:H11"/>
@@ -2064,25 +1975,6 @@
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="K21:O21"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="L23:O23"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="L25:O25"/>
-    <mergeCell ref="L26:O26"/>
-    <mergeCell ref="L27:O27"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added headers to input lists
</commit_message>
<xml_diff>
--- a/Input List/Acoustic/Input List.xlsx
+++ b/Input List/Acoustic/Input List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Input List\Acoustic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED9D0E0-347C-4FBD-A8C4-E19E40FFAF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455BEB07-7C65-4A5E-A89D-0B8B916878F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Input + Equipment" sheetId="1" r:id="rId1"/>
@@ -36,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="67">
   <si>
     <t>Input</t>
   </si>
@@ -232,13 +254,19 @@
   </si>
   <si>
     <t>EQ up lower and mid. Lots of reverb.</t>
+  </si>
+  <si>
+    <t>Acoustic Setup</t>
+  </si>
+  <si>
+    <t>www.theperfectstrangers.band</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,8 +388,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,12 +424,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -412,18 +442,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF66CCFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCECFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -437,18 +455,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF15B1FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -482,8 +488,20 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA3E0FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE5F5FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -546,27 +564,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -579,10 +604,9 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -591,77 +615,95 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -704,13 +746,20 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="1"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -719,22 +768,28 @@
         </right>
         <top/>
         <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00E266"/>
+      <color rgb="FFE5F5FF"/>
+      <color rgb="FFA3E0FF"/>
       <color rgb="FFFF00FF"/>
       <color rgb="FF0000FF"/>
       <color rgb="FF0066FF"/>
-      <color rgb="FF00E266"/>
       <color rgb="FF00B050"/>
       <color rgb="FF6188CD"/>
       <color rgb="FF15B1FF"/>
       <color rgb="FF4572C3"/>
-      <color rgb="FF00B6F6"/>
-      <color rgb="FF7193D1"/>
     </mruColors>
   </colors>
   <extLst>
@@ -748,9 +803,73 @@
 </styleSheet>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+</richValueRels>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4F9D055F-F885-4EC9-A0D7-7F756C0DE538}" name="Table2" displayName="Table2" ref="K2:L18" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="K2:L18" xr:uid="{4F9D055F-F885-4EC9-A0D7-7F756C0DE538}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4F9D055F-F885-4EC9-A0D7-7F756C0DE538}" name="Table2" displayName="Table2" ref="K4:L20" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2">
+  <autoFilter ref="K4:L20" xr:uid="{4F9D055F-F885-4EC9-A0D7-7F756C0DE538}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{49BF8DF2-5386-41E7-B011-F853E4FE75C2}" name="Channel" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{85FAB182-B344-4EA5-B466-95EC3E4BC71D}" name="Name" dataDxfId="0"/>
@@ -760,9 +879,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -800,7 +919,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -906,7 +1025,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1048,7 +1167,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1056,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A11D25-D77D-4358-9E34-E04B11CA4C7B}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,355 +1194,379 @@
     <col min="9" max="21" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+    </row>
+    <row r="2" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H3" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B4" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C4" s="23">
         <v>1</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E4" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F4" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18" t="s">
+      <c r="G4" s="23"/>
+      <c r="H4" s="23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="3">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="3">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="18">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="23">
         <v>3</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D6" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E6" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F6" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18" t="s">
+      <c r="G6" s="23"/>
+      <c r="H6" s="23" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="10">
-        <v>4</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="11">
-        <v>5</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="7">
-        <v>6</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="8">
+        <v>4</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7" t="s">
-        <v>63</v>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28"/>
       <c r="B8" s="29"/>
-      <c r="C8" s="8">
+      <c r="C8" s="9">
+        <v>5</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="24">
+        <v>6</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="25">
         <v>7</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D10" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E10" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F10" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="7">
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="24">
         <v>8</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D11" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E11" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F11" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B12" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C12" s="18">
         <v>9</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E12" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F12" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21" t="s">
+      <c r="G12" s="18"/>
+      <c r="H12" s="18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="9">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="37"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="7">
         <v>10</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B14" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C14" s="4">
         <v>11</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4" t="s">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="5">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="5">
         <v>12</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="4">
-        <v>13</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="5">
-        <v>14</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>44</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="19">
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="4">
+        <v>13</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="5">
+        <v>14</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="16">
         <v>15</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D18" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B19" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C19" s="17">
         <v>16</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D19" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E19" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F19" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+    </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1432,19 +1575,24 @@
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="D16:H16"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
+  <mergeCells count="14">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:E2"/>
+    <mergeCell ref="F1:H2"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1454,10 +1602,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036672A4-8952-44C6-9E0D-0D4906E8D835}">
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,506 +1623,549 @@
     <col min="19" max="19" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+    </row>
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+    </row>
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="15"/>
-      <c r="K1" s="44" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="13"/>
+      <c r="K3" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="44"/>
-    </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="L3" s="52"/>
+    </row>
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="15"/>
-      <c r="K2" s="22" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="13"/>
+      <c r="K4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L4" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="O2" s="12"/>
-    </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="O4" s="10"/>
+    </row>
+    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B5" s="12">
         <v>2</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C5" s="12">
         <v>3</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D5" s="12">
         <v>4</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E5" s="12">
         <v>5</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F5" s="12">
         <v>6</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G5" s="12">
         <v>7</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H5" s="12">
         <v>8</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="K3" s="18">
+      <c r="I5" s="13"/>
+      <c r="K5" s="23">
         <v>1</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="L5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="12"/>
-    </row>
-    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="O5" s="10"/>
+    </row>
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B6" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C6" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D6" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E6" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F6" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G6" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H6" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="K4" s="3">
+      <c r="I6" s="13"/>
+      <c r="K6" s="3">
         <v>2</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O4" s="12"/>
-    </row>
-    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="15"/>
-      <c r="K5" s="18">
+      <c r="O6" s="10"/>
+    </row>
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="42"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="13"/>
+      <c r="K7" s="23">
         <v>3</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="L7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="O5" s="12"/>
-    </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I6" s="15"/>
-      <c r="K6" s="10">
+      <c r="O7" s="10"/>
+    </row>
+    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="13"/>
+      <c r="K8" s="8">
         <v>4</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="12"/>
-    </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="O8" s="10"/>
+    </row>
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
         <v>9</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B9" s="12">
         <v>10</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C9" s="12">
         <v>11</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D9" s="12">
         <v>12</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E9" s="12">
         <v>13</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F9" s="12">
         <v>14</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G9" s="12">
         <v>15</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H9" s="12">
         <v>16</v>
       </c>
-      <c r="I7" s="15"/>
-      <c r="K7" s="11">
+      <c r="I9" s="13"/>
+      <c r="K9" s="9">
         <v>5</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="L9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="O7" s="12"/>
-    </row>
-    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="O9" s="10"/>
+    </row>
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B10" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C10" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D10" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E10" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F10" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="36"/>
-      <c r="H8" s="42" t="s">
+      <c r="G10" s="49"/>
+      <c r="H10" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="15"/>
-      <c r="K8" s="7">
+      <c r="I10" s="13"/>
+      <c r="K10" s="24">
         <v>6</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L10" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="O8" s="12"/>
-    </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="15"/>
-      <c r="K9" s="8">
+      <c r="O10" s="10"/>
+    </row>
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="46"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="13"/>
+      <c r="K11" s="25">
         <v>7</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="L11" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="12"/>
-    </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I10" s="15"/>
-      <c r="K10" s="7">
+      <c r="O11" s="10"/>
+    </row>
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="13"/>
+      <c r="K12" s="24">
         <v>8</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L12" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="O10" s="12"/>
-    </row>
-    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="O12" s="10"/>
+    </row>
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="15"/>
-      <c r="K11" s="21">
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="13"/>
+      <c r="K13" s="18">
         <v>9</v>
       </c>
-      <c r="L11" s="21" t="s">
+      <c r="L13" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="O11" s="12"/>
-    </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
+      <c r="O13" s="10"/>
+    </row>
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <v>1</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B14" s="12">
         <v>2</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C14" s="12">
         <v>3</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D14" s="12">
         <v>4</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E14" s="12">
         <v>5</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F14" s="12">
         <v>6</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G14" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H14" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="I12" s="15"/>
-      <c r="K12" s="9">
+      <c r="I14" s="13"/>
+      <c r="K14" s="7">
         <v>10</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="L14" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="O12" s="12"/>
-    </row>
-    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="42" t="s">
+      <c r="O14" s="10"/>
+    </row>
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="49"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="42" t="s">
+      <c r="H15" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="I13" s="15"/>
-      <c r="K13" s="4">
+      <c r="I15" s="13"/>
+      <c r="K15" s="4">
         <v>11</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="O13" s="12"/>
-    </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="15"/>
-      <c r="K14" s="5">
+      <c r="O15" s="10"/>
+    </row>
+    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="49"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="13"/>
+      <c r="K16" s="5">
         <v>12</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="L16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="O14" s="12"/>
-    </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="15"/>
-      <c r="K15" s="4">
+      <c r="O16" s="10"/>
+    </row>
+    <row r="17" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="13"/>
+      <c r="K17" s="4">
         <v>13</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L17" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="O15" s="12"/>
-    </row>
-    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I16" s="15"/>
-      <c r="K16" s="5">
+      <c r="O17" s="10"/>
+    </row>
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="13"/>
+      <c r="K18" s="5">
         <v>14</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="O16" s="12"/>
-    </row>
-    <row r="17" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I17" s="15"/>
-      <c r="K17" s="19">
+      <c r="O18" s="10"/>
+    </row>
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="13"/>
+      <c r="K19" s="16">
         <v>15</v>
       </c>
-      <c r="L17" s="23" t="s">
+      <c r="L19" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="O17" s="12"/>
-    </row>
-    <row r="18" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I18" s="15"/>
-      <c r="K18" s="19">
+      <c r="O19" s="10"/>
+    </row>
+    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="13"/>
+      <c r="K20" s="16">
         <v>16</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="L20" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="O18" s="12"/>
-    </row>
-    <row r="19" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" spans="9:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I20" s="15"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-    </row>
-    <row r="21" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I21" s="15"/>
-      <c r="K21" s="45" t="s">
+      <c r="O20" s="10"/>
+    </row>
+    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="13"/>
+    </row>
+    <row r="22" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I22" s="13"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="13"/>
+      <c r="K23" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="45"/>
-    </row>
-    <row r="22" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I22" s="15"/>
-      <c r="K22" s="6">
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="50"/>
+    </row>
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="13"/>
+      <c r="K24" s="6">
         <v>1</v>
       </c>
-      <c r="L22" s="46" t="s">
+      <c r="L24" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="M22" s="46"/>
-      <c r="N22" s="46"/>
-      <c r="O22" s="46"/>
-    </row>
-    <row r="23" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I23" s="15"/>
-      <c r="K23" s="2">
+      <c r="M24" s="48"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="48"/>
+    </row>
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="13"/>
+      <c r="K25" s="2">
         <v>2</v>
       </c>
-      <c r="L23" s="47" t="s">
+      <c r="L25" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="47"/>
-    </row>
-    <row r="24" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I24" s="15"/>
-      <c r="K24" s="6">
-        <v>3</v>
-      </c>
-      <c r="L24" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="46"/>
-    </row>
-    <row r="25" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I25" s="15"/>
-      <c r="K25" s="2">
-        <v>4</v>
-      </c>
-      <c r="L25" s="47"/>
       <c r="M25" s="47"/>
       <c r="N25" s="47"/>
       <c r="O25" s="47"/>
     </row>
-    <row r="26" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I26" s="15"/>
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="13"/>
       <c r="K26" s="6">
-        <v>5</v>
-      </c>
-      <c r="L26" s="46"/>
-      <c r="M26" s="46"/>
-      <c r="N26" s="46"/>
-      <c r="O26" s="46"/>
-    </row>
-    <row r="27" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I27" s="15"/>
+        <v>3</v>
+      </c>
+      <c r="L26" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="M26" s="48"/>
+      <c r="N26" s="48"/>
+      <c r="O26" s="48"/>
+    </row>
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I27" s="13"/>
       <c r="K27" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L27" s="47"/>
       <c r="M27" s="47"/>
       <c r="N27" s="47"/>
       <c r="O27" s="47"/>
     </row>
-    <row r="28" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="13"/>
+      <c r="K28" s="6">
+        <v>5</v>
+      </c>
+      <c r="L28" s="48"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="48"/>
+      <c r="O28" s="48"/>
+    </row>
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="13"/>
+      <c r="K29" s="2">
+        <v>6</v>
+      </c>
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="47"/>
+    </row>
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
+  <mergeCells count="38">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:J2"/>
+    <mergeCell ref="K1:O2"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="L24:O24"/>
     <mergeCell ref="L25:O25"/>
     <mergeCell ref="L26:O26"/>
-    <mergeCell ref="L27:O27"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="K21:O21"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="L23:O23"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed acoustic input names
</commit_message>
<xml_diff>
--- a/Input List/Acoustic/Input List.xlsx
+++ b/Input List/Acoustic/Input List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Input List\Acoustic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455BEB07-7C65-4A5E-A89D-0B8B916878F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350D6758-3411-4197-841D-F58D2ADD6547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Input + Equipment" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
   <si>
     <t>Input</t>
   </si>
@@ -67,18 +67,12 @@
     <t>Paul Vocals</t>
   </si>
   <si>
-    <t>Paul Electric</t>
-  </si>
-  <si>
     <t>Kenzi Vocals</t>
   </si>
   <si>
     <t>Kenzi Keys</t>
   </si>
   <si>
-    <t>Kenzi Acstc</t>
-  </si>
-  <si>
     <t>Output</t>
   </si>
   <si>
@@ -208,15 +202,9 @@
     <t>16-Channel Split</t>
   </si>
   <si>
-    <t>Jessica Acstc</t>
-  </si>
-  <si>
     <t>Black cables = utility (PA and patching)</t>
   </si>
   <si>
-    <t>Bongos</t>
-  </si>
-  <si>
     <t>Shure SM57</t>
   </si>
   <si>
@@ -260,13 +248,34 @@
   </si>
   <si>
     <t>www.theperfectstrangers.band</t>
+  </si>
+  <si>
+    <t>Chad Monitor</t>
+  </si>
+  <si>
+    <t>John Monitor</t>
+  </si>
+  <si>
+    <t>Paul Monitor</t>
+  </si>
+  <si>
+    <t>Kenzi Monitor</t>
+  </si>
+  <si>
+    <t>Vocal Sub Group</t>
+  </si>
+  <si>
+    <t>Chad Bongos</t>
+  </si>
+  <si>
+    <t>Jessica Monitor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,6 +405,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="18">
     <fill>
@@ -501,7 +524,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -573,11 +596,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -618,6 +652,33 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -636,69 +697,46 @@
     <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1177,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A11D25-D77D-4358-9E34-E04B11CA4C7B}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,227 +1233,227 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="e" vm="1">
+      <c r="A1" s="26" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="11" t="s">
+      <c r="H3" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="34" t="s">
         <v>14</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="23">
         <v>1</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G4" s="23"/>
       <c r="H4" s="23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="40"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="3">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="40"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="23">
         <v>3</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G6" s="23"/>
       <c r="H6" s="23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>28</v>
+      <c r="A7" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>26</v>
       </c>
       <c r="C7" s="8">
         <v>4</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="9">
         <v>5</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>44</v>
-      </c>
       <c r="F8" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>22</v>
+      <c r="A9" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>20</v>
       </c>
       <c r="C9" s="24">
         <v>6</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G9" s="24"/>
       <c r="H9" s="24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="31"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="40"/>
       <c r="C10" s="25">
         <v>7</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="31"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="24">
         <v>8</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>27</v>
+      <c r="A12" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>25</v>
       </c>
       <c r="C12" s="18">
         <v>9</v>
@@ -1424,108 +1462,108 @@
         <v>1</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G12" s="18"/>
       <c r="H12" s="18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
-      <c r="B13" s="38"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="7">
         <v>10</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>23</v>
+      <c r="A14" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C14" s="4">
         <v>11</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="5">
         <v>12</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="4">
         <v>13</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="5">
         <v>14</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -1536,32 +1574,32 @@
       <c r="C18" s="16">
         <v>15</v>
       </c>
-      <c r="D18" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
+      <c r="D18" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C19" s="17">
         <v>16</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
@@ -1579,6 +1617,13 @@
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:E2"/>
     <mergeCell ref="F1:H2"/>
@@ -1586,13 +1631,6 @@
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="D18:H18"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1604,8 +1642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036672A4-8952-44C6-9E0D-0D4906E8D835}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="S35" sqref="S35"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,79 +1662,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="e" vm="1">
+      <c r="A1" s="26" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
+      <c r="A3" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
       <c r="I3" s="13"/>
-      <c r="K3" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="L3" s="52"/>
+      <c r="K3" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="41"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
       <c r="I4" s="13"/>
       <c r="K4" s="19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O4" s="10"/>
     </row>
@@ -1730,59 +1768,59 @@
         <v>1</v>
       </c>
       <c r="L5" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" s="10"/>
+    </row>
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="10"/>
-    </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="44" t="s">
-        <v>43</v>
+      <c r="H6" s="50" t="s">
+        <v>41</v>
       </c>
       <c r="I6" s="13"/>
       <c r="K6" s="3">
         <v>2</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="O6" s="10"/>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
       <c r="I7" s="13"/>
       <c r="K7" s="23">
         <v>3</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="O7" s="10"/>
     </row>
@@ -1792,7 +1830,7 @@
         <v>4</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O8" s="10"/>
     </row>
@@ -1826,7 +1864,7 @@
         <v>5</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O9" s="10"/>
     </row>
@@ -1835,30 +1873,30 @@
         <v>1</v>
       </c>
       <c r="B10" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="D10" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="49"/>
-      <c r="H10" s="45" t="s">
-        <v>55</v>
+      <c r="G10" s="48"/>
+      <c r="H10" s="53" t="s">
+        <v>51</v>
       </c>
       <c r="I10" s="13"/>
       <c r="K10" s="24">
         <v>6</v>
       </c>
       <c r="L10" s="24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O10" s="10"/>
     </row>
@@ -1869,14 +1907,14 @@
       <c r="D11" s="51"/>
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="45"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="53"/>
       <c r="I11" s="13"/>
       <c r="K11" s="25">
         <v>7</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O11" s="10"/>
     </row>
@@ -1886,21 +1924,21 @@
         <v>8</v>
       </c>
       <c r="L12" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O12" s="10"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
+      <c r="A13" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
       <c r="I13" s="13"/>
       <c r="K13" s="18">
         <v>9</v>
@@ -1930,57 +1968,69 @@
         <v>6</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I14" s="13"/>
       <c r="K14" s="7">
         <v>10</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="O14" s="10"/>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15" s="45" t="s">
-        <v>58</v>
+      <c r="A15" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="53" t="s">
+        <v>54</v>
       </c>
       <c r="I15" s="13"/>
       <c r="K15" s="4">
         <v>11</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O15" s="10"/>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
       <c r="I16" s="13"/>
       <c r="K16" s="5">
         <v>12</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O16" s="10"/>
     </row>
@@ -1993,12 +2043,12 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="13"/>
+      <c r="I17" s="54"/>
       <c r="K17" s="4">
         <v>13</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O17" s="10"/>
     </row>
@@ -2008,7 +2058,7 @@
         <v>14</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O18" s="10"/>
     </row>
@@ -2018,7 +2068,7 @@
         <v>15</v>
       </c>
       <c r="L19" s="20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="O19" s="10"/>
     </row>
@@ -2028,7 +2078,7 @@
         <v>16</v>
       </c>
       <c r="L20" s="20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="O20" s="10"/>
     </row>
@@ -2046,79 +2096,79 @@
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I23" s="13"/>
-      <c r="K23" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="50"/>
+      <c r="K23" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="44"/>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I24" s="13"/>
       <c r="K24" s="6">
         <v>1</v>
       </c>
-      <c r="L24" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="M24" s="48"/>
-      <c r="N24" s="48"/>
-      <c r="O24" s="48"/>
+      <c r="L24" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I25" s="13"/>
       <c r="K25" s="2">
         <v>2</v>
       </c>
-      <c r="L25" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
-      <c r="O25" s="47"/>
+      <c r="L25" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I26" s="13"/>
       <c r="K26" s="6">
         <v>3</v>
       </c>
-      <c r="L26" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="M26" s="48"/>
-      <c r="N26" s="48"/>
-      <c r="O26" s="48"/>
+      <c r="L26" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I27" s="13"/>
       <c r="K27" s="2">
         <v>4</v>
       </c>
-      <c r="L27" s="47"/>
-      <c r="M27" s="47"/>
-      <c r="N27" s="47"/>
-      <c r="O27" s="47"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="42"/>
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I28" s="13"/>
       <c r="K28" s="6">
         <v>5</v>
       </c>
-      <c r="L28" s="48"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="48"/>
-      <c r="O28" s="48"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="43"/>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I29" s="13"/>
       <c r="K29" s="2">
         <v>6</v>
       </c>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="47"/>
-      <c r="O29" s="47"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="42"/>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2128,30 +2178,6 @@
     <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:J2"/>
-    <mergeCell ref="K1:O2"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="L29:O29"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="K23:O23"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="L25:O25"/>
-    <mergeCell ref="L26:O26"/>
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:H4"/>
@@ -2166,6 +2192,30 @@
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:J2"/>
+    <mergeCell ref="K1:O2"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="F10:F11"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated split names and colors
</commit_message>
<xml_diff>
--- a/Input List/Acoustic/Input List.xlsx
+++ b/Input List/Acoustic/Input List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\TechnicalDocumentation\Input List\Acoustic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Input List\Acoustic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51433ABC-3C30-4218-858D-07FF07353860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98BD934-809D-432E-BC23-1CC0A5E9F458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Input + Equipment" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t>Input</t>
   </si>
@@ -230,9 +230,6 @@
   </si>
   <si>
     <t>Group Monitor</t>
-  </si>
-  <si>
-    <t>Acoustic Setup 1.0</t>
   </si>
   <si>
     <t>Position</t>
@@ -276,6 +273,54 @@
   </si>
   <si>
     <t>Kenzi Acstc</t>
+  </si>
+  <si>
+    <t>DSR Vocals</t>
+  </si>
+  <si>
+    <t>DSR Bass</t>
+  </si>
+  <si>
+    <t>DSR Aux</t>
+  </si>
+  <si>
+    <t>DCR Vocals</t>
+  </si>
+  <si>
+    <t>DCL Vocals</t>
+  </si>
+  <si>
+    <t>DCR Acstc Gtr</t>
+  </si>
+  <si>
+    <t>DCL Elec Gtr</t>
+  </si>
+  <si>
+    <t>DCL Acstc Gtr</t>
+  </si>
+  <si>
+    <t>DSL Vocals</t>
+  </si>
+  <si>
+    <t>DSL Acstc Gtr</t>
+  </si>
+  <si>
+    <t>DSL Piano</t>
+  </si>
+  <si>
+    <t>DSL Keyboard</t>
+  </si>
+  <si>
+    <t>USC Vocals</t>
+  </si>
+  <si>
+    <t>USC Bongos</t>
+  </si>
+  <si>
+    <t>USC Aux</t>
+  </si>
+  <si>
+    <t>Acoustic Setup 1.1</t>
   </si>
 </sst>
 </file>
@@ -691,6 +736,20 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -706,13 +765,58 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -742,82 +846,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1299,7 +1346,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,37 +1363,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="e" vm="1">
+      <c r="A1" s="31" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="29" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>9</v>
@@ -1368,11 +1415,11 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>59</v>
+      <c r="A4" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>58</v>
       </c>
       <c r="C4" s="20">
         <v>1</v>
@@ -1392,8 +1439,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
-      <c r="B5" s="48"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="3">
         <v>2</v>
       </c>
@@ -1410,8 +1457,8 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="58"/>
-      <c r="B6" s="48"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="20">
         <v>3</v>
       </c>
@@ -1430,11 +1477,11 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="59" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="49" t="s">
-        <v>60</v>
+      <c r="A7" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>59</v>
       </c>
       <c r="C7" s="21">
         <v>6</v>
@@ -1454,8 +1501,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="50"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="22">
         <v>7</v>
       </c>
@@ -1472,8 +1519,8 @@
       <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="21">
         <v>8</v>
       </c>
@@ -1490,11 +1537,11 @@
       <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="60" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="51" t="s">
-        <v>61</v>
+      <c r="A10" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>60</v>
       </c>
       <c r="C10" s="7">
         <v>4</v>
@@ -1514,8 +1561,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="60"/>
-      <c r="B11" s="51"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="44"/>
       <c r="C11" s="8">
         <v>5</v>
       </c>
@@ -1532,32 +1579,32 @@
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="67">
+      <c r="A12" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="26">
         <v>9</v>
       </c>
-      <c r="D12" s="67" t="s">
+      <c r="D12" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="67" t="s">
+      <c r="E12" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="67" t="s">
+      <c r="F12" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67" t="s">
+      <c r="G12" s="26"/>
+      <c r="H12" s="26" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="62"/>
-      <c r="B13" s="53"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="6">
         <v>10</v>
       </c>
@@ -1574,50 +1621,50 @@
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="63"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="67">
+      <c r="A14" s="47"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="26">
         <v>11</v>
       </c>
-      <c r="D14" s="67" t="s">
+      <c r="D14" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="67" t="s">
+      <c r="E14" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="67" t="s">
+      <c r="F14" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="66">
+      <c r="A15" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="25">
         <v>11</v>
       </c>
-      <c r="D15" s="66" t="s">
+      <c r="D15" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="66" t="s">
+      <c r="E15" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="66" t="s">
+      <c r="F15" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="66"/>
-      <c r="H15" s="66" t="s">
+      <c r="G15" s="25"/>
+      <c r="H15" s="25" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="56"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="4">
         <v>12</v>
       </c>
@@ -1634,26 +1681,26 @@
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="66">
+      <c r="A17" s="28"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="25">
         <v>13</v>
       </c>
-      <c r="D17" s="66" t="s">
+      <c r="D17" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="66" t="s">
+      <c r="E17" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="66" t="s">
+      <c r="F17" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="56"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="4">
         <v>14</v>
       </c>
@@ -1704,12 +1751,6 @@
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="B15:B18"/>
     <mergeCell ref="A1:B2"/>
@@ -1717,6 +1758,12 @@
     <mergeCell ref="F1:H2"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1728,8 +1775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036672A4-8952-44C6-9E0D-0D4906E8D835}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1748,73 +1795,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="e" vm="1">
+      <c r="A1" s="31" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="29" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
       <c r="I3" s="12"/>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="33"/>
+      <c r="L3" s="54"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
       <c r="I4" s="12"/>
       <c r="K4" s="17" t="s">
         <v>9</v>
@@ -1853,32 +1900,32 @@
         <v>1</v>
       </c>
       <c r="L5" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="67" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="32" t="s">
+      <c r="H6" s="63" t="s">
         <v>38</v>
       </c>
       <c r="I6" s="12"/>
@@ -1886,33 +1933,33 @@
         <v>2</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
+      <c r="A7" s="68"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
       <c r="I7" s="12"/>
       <c r="K7" s="21">
         <v>3</v>
       </c>
       <c r="L7" s="21" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I8" s="12"/>
-      <c r="K8" s="65">
+      <c r="K8" s="7">
         <v>4</v>
       </c>
-      <c r="L8" s="65" t="s">
-        <v>26</v>
+      <c r="L8" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1941,89 +1988,89 @@
         <v>16</v>
       </c>
       <c r="I9" s="12"/>
-      <c r="K9" s="65">
+      <c r="K9" s="7">
         <v>5</v>
       </c>
-      <c r="L9" s="65" t="s">
-        <v>29</v>
+      <c r="L9" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="68" t="s">
+      <c r="B10" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="68" t="s">
+      <c r="D10" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="43" t="s">
+      <c r="F10" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="43" t="s">
+      <c r="G10" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="H10" s="61" t="s">
         <v>40</v>
       </c>
       <c r="I10" s="12"/>
-      <c r="K10" s="67">
+      <c r="K10" s="26">
         <v>6</v>
       </c>
-      <c r="L10" s="67" t="s">
-        <v>1</v>
+      <c r="L10" s="26" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="69"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="40"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="61"/>
       <c r="I11" s="12"/>
-      <c r="K11" s="67">
+      <c r="K11" s="26">
         <v>7</v>
       </c>
-      <c r="L11" s="67" t="s">
-        <v>53</v>
+      <c r="L11" s="26" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I12" s="12"/>
-      <c r="K12" s="67">
+      <c r="K12" s="26">
         <v>8</v>
       </c>
-      <c r="L12" s="67" t="s">
-        <v>38</v>
+      <c r="L12" s="26" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
       <c r="I13" s="12"/>
-      <c r="K13" s="66">
+      <c r="K13" s="25">
         <v>9</v>
       </c>
-      <c r="L13" s="66" t="s">
-        <v>2</v>
+      <c r="L13" s="25" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2052,54 +2099,54 @@
         <v>43</v>
       </c>
       <c r="I14" s="12"/>
-      <c r="K14" s="66">
+      <c r="K14" s="25">
         <v>10</v>
       </c>
-      <c r="L14" s="66" t="s">
-        <v>24</v>
+      <c r="L14" s="25" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="39" t="s">
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="40" t="s">
+      <c r="G15" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="40" t="s">
+      <c r="H15" s="61" t="s">
         <v>43</v>
       </c>
       <c r="I15" s="12"/>
-      <c r="K15" s="66">
+      <c r="K15" s="25">
         <v>11</v>
       </c>
-      <c r="L15" s="66" t="s">
-        <v>44</v>
+      <c r="L15" s="25" t="s">
+        <v>79</v>
       </c>
       <c r="O15" s="9"/>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
       <c r="I16" s="12"/>
-      <c r="K16" s="66">
+      <c r="K16" s="25">
         <v>12</v>
       </c>
-      <c r="L16" s="66" t="s">
-        <v>3</v>
+      <c r="L16" s="25" t="s">
+        <v>80</v>
       </c>
       <c r="O16" s="9"/>
     </row>
@@ -2117,7 +2164,7 @@
         <v>13</v>
       </c>
       <c r="L17" s="20" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="O17" s="9"/>
     </row>
@@ -2128,7 +2175,7 @@
         <v>14</v>
       </c>
       <c r="L18" s="20" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="O18" s="9"/>
     </row>
@@ -2138,7 +2185,7 @@
         <v>15</v>
       </c>
       <c r="L19" s="20" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="O19" s="9"/>
     </row>
@@ -2166,79 +2213,79 @@
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I23" s="12"/>
-      <c r="K23" s="41" t="s">
+      <c r="K23" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
+      <c r="N23" s="62"/>
+      <c r="O23" s="62"/>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I24" s="12"/>
       <c r="K24" s="5">
         <v>1</v>
       </c>
-      <c r="L24" s="38" t="s">
+      <c r="L24" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="M24" s="38"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
+      <c r="M24" s="59"/>
+      <c r="N24" s="59"/>
+      <c r="O24" s="59"/>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I25" s="12"/>
       <c r="K25" s="2">
         <v>2</v>
       </c>
-      <c r="L25" s="37" t="s">
+      <c r="L25" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="M25" s="37"/>
-      <c r="N25" s="37"/>
-      <c r="O25" s="37"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="58"/>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I26" s="12"/>
       <c r="K26" s="5">
         <v>3</v>
       </c>
-      <c r="L26" s="38" t="s">
+      <c r="L26" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
-      <c r="O26" s="38"/>
+      <c r="M26" s="59"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="59"/>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I27" s="12"/>
       <c r="K27" s="2">
         <v>4</v>
       </c>
-      <c r="L27" s="37"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="37"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="58"/>
+      <c r="N27" s="58"/>
+      <c r="O27" s="58"/>
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I28" s="12"/>
       <c r="K28" s="5">
         <v>5</v>
       </c>
-      <c r="L28" s="38"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="38"/>
-      <c r="O28" s="38"/>
+      <c r="L28" s="59"/>
+      <c r="M28" s="59"/>
+      <c r="N28" s="59"/>
+      <c r="O28" s="59"/>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I29" s="12"/>
       <c r="K29" s="2">
         <v>6</v>
       </c>
-      <c r="L29" s="37"/>
-      <c r="M29" s="37"/>
-      <c r="N29" s="37"/>
-      <c r="O29" s="37"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="58"/>
+      <c r="N29" s="58"/>
+      <c r="O29" s="58"/>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2248,22 +2295,11 @@
     <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H4"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H10:H11"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="D6:D7"/>
     <mergeCell ref="L27:O27"/>
     <mergeCell ref="L28:O28"/>
     <mergeCell ref="L29:O29"/>
@@ -2279,6 +2315,17 @@
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:J2"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:H4"/>
     <mergeCell ref="K1:O2"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>

</xml_diff>

<commit_message>
Updated all flows to use new install path
</commit_message>
<xml_diff>
--- a/Input List/Acoustic/Input List.xlsx
+++ b/Input List/Acoustic/Input List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Input List\Acoustic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\TechnicalDocumentation\Input List\Acoustic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1A75E5-F35A-4D43-84A2-E1D6E5FDE74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE74E8C0-0508-4157-A2C0-13F0B5697D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Input + Equipment" sheetId="1" r:id="rId1"/>
@@ -744,6 +744,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -804,6 +818,54 @@
     <xf numFmtId="0" fontId="18" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -811,68 +873,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1371,30 +1371,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="e" vm="1">
+      <c r="A1" s="31" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="27" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="29" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -1423,10 +1423,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="38" t="s">
         <v>58</v>
       </c>
       <c r="C4" s="19">
@@ -1447,8 +1447,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="3">
         <v>2</v>
       </c>
@@ -1465,8 +1465,8 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="B6" s="32"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="19">
         <v>3</v>
       </c>
@@ -1485,10 +1485,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="41" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="20">
@@ -1509,8 +1509,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="36"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="21">
         <v>7</v>
       </c>
@@ -1527,8 +1527,8 @@
       <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="36"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="20">
         <v>8</v>
       </c>
@@ -1545,10 +1545,10 @@
       <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="44" t="s">
         <v>60</v>
       </c>
       <c r="C10" s="6">
@@ -1569,8 +1569,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="38"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="44"/>
       <c r="C11" s="7">
         <v>5</v>
       </c>
@@ -1587,10 +1587,10 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="48" t="s">
         <v>61</v>
       </c>
       <c r="C12" s="24">
@@ -1611,8 +1611,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="43"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="5">
         <v>10</v>
       </c>
@@ -1629,8 +1629,8 @@
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="44"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="24">
         <v>11</v>
       </c>
@@ -1647,82 +1647,82 @@
       <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="67">
+      <c r="C15" s="26">
         <v>11</v>
       </c>
-      <c r="D15" s="67" t="s">
+      <c r="D15" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="67" t="s">
+      <c r="E15" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="67" t="s">
+      <c r="F15" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67" t="s">
+      <c r="G15" s="26"/>
+      <c r="H15" s="26" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="65"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="62">
+      <c r="A16" s="28"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="25">
         <v>12</v>
       </c>
-      <c r="D16" s="62" t="s">
+      <c r="D16" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="62" t="s">
+      <c r="E16" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="62" t="s">
+      <c r="F16" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="65"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="67">
+      <c r="A17" s="28"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="26">
         <v>13</v>
       </c>
-      <c r="D17" s="67" t="s">
+      <c r="D17" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="67" t="s">
+      <c r="E17" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="67" t="s">
+      <c r="F17" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="65"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="62">
+      <c r="A18" s="28"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="25">
         <v>14</v>
       </c>
-      <c r="D18" s="62" t="s">
+      <c r="D18" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="62" t="s">
+      <c r="E18" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="62" t="s">
+      <c r="F18" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="62"/>
-      <c r="H18" s="62"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
@@ -1784,7 +1784,7 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1803,73 +1803,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="e" vm="1">
+      <c r="A1" s="31" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="27" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="29" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
       <c r="I3" s="11"/>
-      <c r="K3" s="61" t="s">
+      <c r="K3" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="61"/>
+      <c r="L3" s="54"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
       <c r="I4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>9</v>
@@ -1912,28 +1912,28 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="58" t="s">
+      <c r="E6" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="56" t="s">
+      <c r="G6" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="56" t="s">
+      <c r="H6" s="58" t="s">
         <v>38</v>
       </c>
       <c r="I6" s="11"/>
@@ -1945,14 +1945,14 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
+      <c r="A7" s="68"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
       <c r="I7" s="11"/>
       <c r="K7" s="20">
         <v>3</v>
@@ -2004,28 +2004,28 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="68" t="s">
+      <c r="D10" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="60" t="s">
+      <c r="F10" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="60" t="s">
+      <c r="G10" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="51" t="s">
+      <c r="H10" s="60" t="s">
         <v>40</v>
       </c>
       <c r="I10" s="11"/>
@@ -2037,14 +2037,14 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="69"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="51"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="60"/>
       <c r="I11" s="11"/>
       <c r="K11" s="24">
         <v>7</v>
@@ -2063,21 +2063,21 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
       <c r="I13" s="11"/>
-      <c r="K13" s="67">
+      <c r="K13" s="26">
         <v>9</v>
       </c>
-      <c r="L13" s="67" t="s">
+      <c r="L13" s="26" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2107,53 +2107,53 @@
         <v>43</v>
       </c>
       <c r="I14" s="11"/>
-      <c r="K14" s="67">
+      <c r="K14" s="26">
         <v>10</v>
       </c>
-      <c r="L14" s="67" t="s">
+      <c r="L14" s="26" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="50" t="s">
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="51" t="s">
+      <c r="G15" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="51" t="s">
+      <c r="H15" s="60" t="s">
         <v>43</v>
       </c>
       <c r="I15" s="11"/>
-      <c r="K15" s="67">
+      <c r="K15" s="26">
         <v>11</v>
       </c>
-      <c r="L15" s="67" t="s">
+      <c r="L15" s="26" t="s">
         <v>79</v>
       </c>
       <c r="O15" s="8"/>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
       <c r="I16" s="11"/>
-      <c r="K16" s="67">
+      <c r="K16" s="26">
         <v>12</v>
       </c>
-      <c r="L16" s="67" t="s">
+      <c r="L16" s="26" t="s">
         <v>80</v>
       </c>
       <c r="O16" s="8"/>
@@ -2221,79 +2221,79 @@
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I23" s="11"/>
-      <c r="K23" s="52" t="s">
+      <c r="K23" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="L23" s="52"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="52"/>
-      <c r="O23" s="52"/>
+      <c r="L23" s="66"/>
+      <c r="M23" s="66"/>
+      <c r="N23" s="66"/>
+      <c r="O23" s="66"/>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I24" s="11"/>
       <c r="K24" s="4">
         <v>1</v>
       </c>
-      <c r="L24" s="49" t="s">
+      <c r="L24" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="49"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="64"/>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I25" s="11"/>
       <c r="K25" s="2">
         <v>2</v>
       </c>
-      <c r="L25" s="48" t="s">
+      <c r="L25" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="M25" s="48"/>
-      <c r="N25" s="48"/>
-      <c r="O25" s="48"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="63"/>
+      <c r="O25" s="63"/>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I26" s="11"/>
       <c r="K26" s="4">
         <v>3</v>
       </c>
-      <c r="L26" s="49" t="s">
+      <c r="L26" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="M26" s="49"/>
-      <c r="N26" s="49"/>
-      <c r="O26" s="49"/>
+      <c r="M26" s="64"/>
+      <c r="N26" s="64"/>
+      <c r="O26" s="64"/>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I27" s="11"/>
       <c r="K27" s="2">
         <v>4</v>
       </c>
-      <c r="L27" s="48"/>
-      <c r="M27" s="48"/>
-      <c r="N27" s="48"/>
-      <c r="O27" s="48"/>
+      <c r="L27" s="63"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="63"/>
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I28" s="11"/>
       <c r="K28" s="4">
         <v>5</v>
       </c>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="49"/>
-      <c r="O28" s="49"/>
+      <c r="L28" s="64"/>
+      <c r="M28" s="64"/>
+      <c r="N28" s="64"/>
+      <c r="O28" s="64"/>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I29" s="11"/>
       <c r="K29" s="2">
         <v>6</v>
       </c>
-      <c r="L29" s="48"/>
-      <c r="M29" s="48"/>
-      <c r="N29" s="48"/>
-      <c r="O29" s="48"/>
+      <c r="L29" s="63"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="63"/>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2303,13 +2303,21 @@
     <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="K1:O2"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="L26:O26"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="E15:E16"/>
@@ -2326,21 +2334,13 @@
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:H4"/>
-    <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="L29:O29"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="K23:O23"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="L25:O25"/>
-    <mergeCell ref="L26:O26"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="K1:O2"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="F10:F11"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added 'Date Updated' to Input Lists
</commit_message>
<xml_diff>
--- a/Input List/Acoustic/Input List.xlsx
+++ b/Input List/Acoustic/Input List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\TechnicalDocumentation\Input List\Acoustic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE74E8C0-0508-4157-A2C0-13F0B5697D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9EA172-F7FD-43D2-9FFC-73E6713B84AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="85">
   <si>
     <t>Input</t>
   </si>
@@ -320,7 +320,7 @@
     <t>USC Aux</t>
   </si>
   <si>
-    <t>Acoustic Setup 1.2</t>
+    <t>Acoustic Setup</t>
   </si>
 </sst>
 </file>
@@ -706,7 +706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -818,62 +818,65 @@
     <xf numFmtId="0" fontId="18" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1354,7 +1357,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F1" sqref="F1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,9 +1395,12 @@
       <c r="C2" s="34"/>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="F2" s="70" t="str">
+        <f ca="1">"Date Updated: "&amp;TEXT(TODAY(),"yyyy-mm-dd")</f>
+        <v>Date Updated: 2024-09-29</v>
+      </c>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -1758,12 +1764,11 @@
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="B15:B18"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:E2"/>
-    <mergeCell ref="F1:H2"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="A7:A9"/>
@@ -1772,6 +1777,8 @@
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="B12:B14"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="F2:H2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1784,7 +1791,7 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1807,8 +1814,9 @@
         <v>#VALUE!</v>
       </c>
       <c r="B1" s="31"/>
-      <c r="C1" s="33" t="s">
-        <v>84</v>
+      <c r="C1" s="33" t="str">
+        <f>'Input + Equipment'!C1</f>
+        <v>Acoustic Setup</v>
       </c>
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
@@ -1817,8 +1825,9 @@
       <c r="H1" s="33"/>
       <c r="I1" s="33"/>
       <c r="J1" s="33"/>
-      <c r="K1" s="35" t="s">
-        <v>50</v>
+      <c r="K1" s="35" t="str">
+        <f>'Input + Equipment'!F1</f>
+        <v>www.theperfectstrangers.band</v>
       </c>
       <c r="L1" s="35"/>
       <c r="M1" s="35"/>
@@ -1836,40 +1845,43 @@
       <c r="H2" s="33"/>
       <c r="I2" s="33"/>
       <c r="J2" s="33"/>
-      <c r="K2" s="35"/>
+      <c r="K2" s="35" t="str">
+        <f ca="1">'Input + Equipment'!F2</f>
+        <v>Date Updated: 2024-09-29</v>
+      </c>
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
       <c r="N2" s="35"/>
       <c r="O2" s="35"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
       <c r="I3" s="11"/>
-      <c r="K3" s="54" t="s">
+      <c r="K3" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="54"/>
+      <c r="L3" s="69"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
       <c r="I4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>9</v>
@@ -1912,28 +1924,28 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="67" t="s">
+      <c r="C6" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="61" t="s">
+      <c r="D6" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="E6" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="58" t="s">
+      <c r="F6" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="58" t="s">
+      <c r="G6" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="58" t="s">
+      <c r="H6" s="64" t="s">
         <v>38</v>
       </c>
       <c r="I6" s="11"/>
@@ -1945,14 +1957,14 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="68"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
       <c r="I7" s="11"/>
       <c r="K7" s="20">
         <v>3</v>
@@ -2004,28 +2016,28 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="53" t="s">
+      <c r="E10" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="53" t="s">
+      <c r="F10" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="53" t="s">
+      <c r="G10" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="60" t="s">
+      <c r="H10" s="59" t="s">
         <v>40</v>
       </c>
       <c r="I10" s="11"/>
@@ -2037,14 +2049,14 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="60"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="59"/>
       <c r="I11" s="11"/>
       <c r="K11" s="24">
         <v>7</v>
@@ -2063,16 +2075,16 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
       <c r="I13" s="11"/>
       <c r="K13" s="26">
         <v>9</v>
@@ -2115,20 +2127,20 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="65" t="s">
+      <c r="B15" s="62"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="60" t="s">
+      <c r="G15" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="60" t="s">
+      <c r="H15" s="59" t="s">
         <v>43</v>
       </c>
       <c r="I15" s="11"/>
@@ -2141,14 +2153,14 @@
       <c r="O15" s="8"/>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
       <c r="I16" s="11"/>
       <c r="K16" s="26">
         <v>12</v>
@@ -2221,79 +2233,79 @@
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I23" s="11"/>
-      <c r="K23" s="66" t="s">
+      <c r="K23" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="L23" s="66"/>
-      <c r="M23" s="66"/>
-      <c r="N23" s="66"/>
-      <c r="O23" s="66"/>
+      <c r="L23" s="60"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="60"/>
+      <c r="O23" s="60"/>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I24" s="11"/>
       <c r="K24" s="4">
         <v>1</v>
       </c>
-      <c r="L24" s="64" t="s">
+      <c r="L24" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="M24" s="64"/>
-      <c r="N24" s="64"/>
-      <c r="O24" s="64"/>
+      <c r="M24" s="57"/>
+      <c r="N24" s="57"/>
+      <c r="O24" s="57"/>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I25" s="11"/>
       <c r="K25" s="2">
         <v>2</v>
       </c>
-      <c r="L25" s="63" t="s">
+      <c r="L25" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="M25" s="63"/>
-      <c r="N25" s="63"/>
-      <c r="O25" s="63"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="56"/>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I26" s="11"/>
       <c r="K26" s="4">
         <v>3</v>
       </c>
-      <c r="L26" s="64" t="s">
+      <c r="L26" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="M26" s="64"/>
-      <c r="N26" s="64"/>
-      <c r="O26" s="64"/>
+      <c r="M26" s="57"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="57"/>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I27" s="11"/>
       <c r="K27" s="2">
         <v>4</v>
       </c>
-      <c r="L27" s="63"/>
-      <c r="M27" s="63"/>
-      <c r="N27" s="63"/>
-      <c r="O27" s="63"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+      <c r="O27" s="56"/>
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I28" s="11"/>
       <c r="K28" s="4">
         <v>5</v>
       </c>
-      <c r="L28" s="64"/>
-      <c r="M28" s="64"/>
-      <c r="N28" s="64"/>
-      <c r="O28" s="64"/>
+      <c r="L28" s="57"/>
+      <c r="M28" s="57"/>
+      <c r="N28" s="57"/>
+      <c r="O28" s="57"/>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I29" s="11"/>
       <c r="K29" s="2">
         <v>6</v>
       </c>
-      <c r="L29" s="63"/>
-      <c r="M29" s="63"/>
-      <c r="N29" s="63"/>
-      <c r="O29" s="63"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="56"/>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2302,22 +2314,15 @@
     <row r="34" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="L29:O29"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="K23:O23"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="L25:O25"/>
-    <mergeCell ref="L26:O26"/>
+  <mergeCells count="39">
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="K2:O2"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="E15:E16"/>
@@ -2334,13 +2339,21 @@
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:H4"/>
-    <mergeCell ref="K1:O2"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>